<commit_message>
Fix mistake in readrules you made on last corrections. had shifted part of a row - so many were out of alignment.
</commit_message>
<xml_diff>
--- a/RULES.xlsx
+++ b/RULES.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="9015" windowHeight="3390"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="9015" windowHeight="3390" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="README" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
     <sheet name="Partsurvey" sheetId="21" r:id="rId21"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">DataDictionary!$A$1:$H$1523</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">DataDictionary!$A$1:$H$1525</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8374" uniqueCount="1435">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8376" uniqueCount="1435">
   <si>
     <t xml:space="preserve">Reminders: </t>
   </si>
@@ -5016,7 +5016,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D1077"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A459" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A459" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="C477" sqref="C477"/>
     </sheetView>
   </sheetViews>
@@ -23752,9 +23752,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H1525"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A1025" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C1038" sqref="C1038"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A1019" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F1039" sqref="F1039"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
@@ -40975,6 +40975,9 @@
       <c r="C1039" t="s">
         <v>10</v>
       </c>
+      <c r="F1039" t="s">
+        <v>1215</v>
+      </c>
     </row>
     <row r="1040" spans="2:6">
       <c r="B1040" t="s">
@@ -40983,6 +40986,9 @@
       <c r="C1040" s="19" t="s">
         <v>12</v>
       </c>
+      <c r="F1040" t="s">
+        <v>1215</v>
+      </c>
     </row>
     <row r="1041" spans="2:6">
       <c r="B1041" t="s">
@@ -41179,9 +41185,6 @@
       <c r="E1054">
         <v>2019</v>
       </c>
-      <c r="F1054" t="s">
-        <v>1215</v>
-      </c>
     </row>
     <row r="1055" spans="2:6">
       <c r="B1055" t="s">
@@ -41196,7 +41199,6 @@
       <c r="E1055">
         <v>2020</v>
       </c>
-      <c r="F1055" s="10"/>
     </row>
     <row r="1056" spans="2:6">
       <c r="B1056" t="s">
@@ -41205,7 +41207,9 @@
       <c r="C1056" s="19" t="s">
         <v>18</v>
       </c>
-      <c r="F1056" s="10"/>
+      <c r="F1056" t="s">
+        <v>1215</v>
+      </c>
     </row>
     <row r="1057" spans="2:7">
       <c r="B1057" t="s">
@@ -41220,12 +41224,7 @@
       <c r="E1057" t="s">
         <v>1236</v>
       </c>
-      <c r="F1057" s="10" t="s">
-        <v>55</v>
-      </c>
-      <c r="G1057" s="10" t="s">
-        <v>1222</v>
-      </c>
+      <c r="F1057" s="10"/>
     </row>
     <row r="1058" spans="2:7">
       <c r="B1058" t="s">
@@ -41240,12 +41239,7 @@
       <c r="E1058" s="10" t="s">
         <v>1238</v>
       </c>
-      <c r="F1058" s="10" t="s">
-        <v>55</v>
-      </c>
-      <c r="G1058" s="10" t="s">
-        <v>1222</v>
-      </c>
+      <c r="F1058" s="10"/>
     </row>
     <row r="1059" spans="2:7">
       <c r="B1059" t="s">
@@ -41254,6 +41248,12 @@
       <c r="C1059" t="s">
         <v>304</v>
       </c>
+      <c r="F1059" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="G1059" s="10" t="s">
+        <v>1222</v>
+      </c>
     </row>
     <row r="1060" spans="2:7">
       <c r="B1060" t="s">
@@ -41262,6 +41262,12 @@
       <c r="C1060" t="s">
         <v>306</v>
       </c>
+      <c r="F1060" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="G1060" s="10" t="s">
+        <v>1222</v>
+      </c>
     </row>
     <row r="1061" spans="2:7">
       <c r="B1061" t="s">
@@ -41276,12 +41282,6 @@
       <c r="E1061" t="s">
         <v>1224</v>
       </c>
-      <c r="F1061" t="s">
-        <v>1230</v>
-      </c>
-      <c r="G1061" t="s">
-        <v>1385</v>
-      </c>
     </row>
     <row r="1062" spans="2:7">
       <c r="B1062" t="s">
@@ -41296,9 +41296,6 @@
       <c r="E1062" t="s">
         <v>1226</v>
       </c>
-      <c r="F1062" t="s">
-        <v>184</v>
-      </c>
     </row>
     <row r="1063" spans="2:7">
       <c r="B1063" t="s">
@@ -41308,7 +41305,10 @@
         <v>22</v>
       </c>
       <c r="F1063" t="s">
-        <v>184</v>
+        <v>1230</v>
+      </c>
+      <c r="G1063" t="s">
+        <v>1385</v>
       </c>
     </row>
     <row r="1064" spans="2:7">
@@ -41374,10 +41374,7 @@
         <v>522</v>
       </c>
       <c r="F1069" t="s">
-        <v>1230</v>
-      </c>
-      <c r="G1069" t="s">
-        <v>1386</v>
+        <v>184</v>
       </c>
     </row>
     <row r="1070" spans="2:7">
@@ -41387,6 +41384,9 @@
       <c r="C1070" t="s">
         <v>524</v>
       </c>
+      <c r="F1070" t="s">
+        <v>184</v>
+      </c>
     </row>
     <row r="1071" spans="2:7">
       <c r="B1071" t="s">
@@ -41395,6 +41395,12 @@
       <c r="C1071" t="s">
         <v>526</v>
       </c>
+      <c r="F1071" t="s">
+        <v>1230</v>
+      </c>
+      <c r="G1071" t="s">
+        <v>1386</v>
+      </c>
     </row>
     <row r="1072" spans="2:7">
       <c r="B1072" t="s">
@@ -41409,9 +41415,6 @@
       <c r="E1072" t="s">
         <v>1236</v>
       </c>
-      <c r="F1072" t="s">
-        <v>184</v>
-      </c>
     </row>
     <row r="1073" spans="2:7">
       <c r="B1073" t="s">
@@ -41426,9 +41429,6 @@
       <c r="E1073" s="10" t="s">
         <v>1238</v>
       </c>
-      <c r="F1073" t="s">
-        <v>184</v>
-      </c>
     </row>
     <row r="1074" spans="2:7">
       <c r="B1074" t="s">
@@ -41438,10 +41438,7 @@
         <v>530</v>
       </c>
       <c r="F1074" t="s">
-        <v>1230</v>
-      </c>
-      <c r="G1074" t="s">
-        <v>1386</v>
+        <v>184</v>
       </c>
     </row>
     <row r="1075" spans="2:7">
@@ -41452,10 +41449,7 @@
         <v>532</v>
       </c>
       <c r="F1075" t="s">
-        <v>1230</v>
-      </c>
-      <c r="G1075" t="s">
-        <v>1386</v>
+        <v>184</v>
       </c>
     </row>
     <row r="1076" spans="2:7">
@@ -41465,6 +41459,12 @@
       <c r="C1076" t="s">
         <v>534</v>
       </c>
+      <c r="F1076" t="s">
+        <v>1230</v>
+      </c>
+      <c r="G1076" t="s">
+        <v>1386</v>
+      </c>
     </row>
     <row r="1077" spans="2:7">
       <c r="B1077" t="s">
@@ -41473,6 +41473,12 @@
       <c r="C1077" t="s">
         <v>536</v>
       </c>
+      <c r="F1077" t="s">
+        <v>1230</v>
+      </c>
+      <c r="G1077" t="s">
+        <v>1386</v>
+      </c>
     </row>
     <row r="1078" spans="2:7">
       <c r="B1078" t="s">
@@ -41487,9 +41493,6 @@
       <c r="E1078" t="s">
         <v>1236</v>
       </c>
-      <c r="F1078" t="s">
-        <v>184</v>
-      </c>
     </row>
     <row r="1079" spans="2:7">
       <c r="B1079" t="s">
@@ -41512,6 +41515,9 @@
       <c r="C1080" t="s">
         <v>540</v>
       </c>
+      <c r="F1080" t="s">
+        <v>184</v>
+      </c>
     </row>
     <row r="1081" spans="2:7">
       <c r="B1081" t="s">
@@ -41526,9 +41532,6 @@
       <c r="E1081" t="s">
         <v>1236</v>
       </c>
-      <c r="F1081" t="s">
-        <v>184</v>
-      </c>
     </row>
     <row r="1082" spans="2:7">
       <c r="B1082" t="s">
@@ -41543,9 +41546,6 @@
       <c r="E1082" s="10" t="s">
         <v>1238</v>
       </c>
-      <c r="F1082" t="s">
-        <v>184</v>
-      </c>
     </row>
     <row r="1083" spans="2:7">
       <c r="B1083" t="s">
@@ -41577,7 +41577,7 @@
         <v>548</v>
       </c>
       <c r="F1085" t="s">
-        <v>1215</v>
+        <v>184</v>
       </c>
     </row>
     <row r="1086" spans="2:7">
@@ -41588,10 +41588,7 @@
         <v>550</v>
       </c>
       <c r="F1086" t="s">
-        <v>1217</v>
-      </c>
-      <c r="G1086" t="s">
-        <v>1218</v>
+        <v>184</v>
       </c>
     </row>
     <row r="1087" spans="2:7">
@@ -41601,11 +41598,8 @@
       <c r="C1087" t="s">
         <v>10</v>
       </c>
-      <c r="F1087" s="10" t="s">
-        <v>55</v>
-      </c>
-      <c r="G1087" s="10" t="s">
-        <v>1222</v>
+      <c r="F1087" t="s">
+        <v>1215</v>
       </c>
     </row>
     <row r="1088" spans="2:7">
@@ -41615,16 +41609,28 @@
       <c r="C1088" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="1089" spans="2:5">
+      <c r="F1088" t="s">
+        <v>1217</v>
+      </c>
+      <c r="G1088" t="s">
+        <v>1218</v>
+      </c>
+    </row>
+    <row r="1089" spans="2:7">
       <c r="B1089" t="s">
         <v>843</v>
       </c>
       <c r="C1089" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="1090" spans="2:5">
+      <c r="F1089" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="G1089" s="10" t="s">
+        <v>1222</v>
+      </c>
+    </row>
+    <row r="1090" spans="2:7">
       <c r="B1090" t="s">
         <v>843</v>
       </c>
@@ -41638,7 +41644,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="1091" spans="2:5">
+    <row r="1091" spans="2:7">
       <c r="B1091" t="s">
         <v>843</v>
       </c>
@@ -41652,7 +41658,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="1092" spans="2:5">
+    <row r="1092" spans="2:7">
       <c r="B1092" t="s">
         <v>843</v>
       </c>
@@ -41666,7 +41672,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="1093" spans="2:5">
+    <row r="1093" spans="2:7">
       <c r="B1093" t="s">
         <v>843</v>
       </c>
@@ -41680,7 +41686,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="1094" spans="2:5">
+    <row r="1094" spans="2:7">
       <c r="B1094" t="s">
         <v>843</v>
       </c>
@@ -41694,7 +41700,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="1095" spans="2:5">
+    <row r="1095" spans="2:7">
       <c r="B1095" t="s">
         <v>843</v>
       </c>
@@ -41708,7 +41714,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="1096" spans="2:5">
+    <row r="1096" spans="2:7">
       <c r="B1096" t="s">
         <v>843</v>
       </c>
@@ -41722,7 +41728,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="1097" spans="2:5">
+    <row r="1097" spans="2:7">
       <c r="B1097" t="s">
         <v>843</v>
       </c>
@@ -41736,7 +41742,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="1098" spans="2:5">
+    <row r="1098" spans="2:7">
       <c r="B1098" t="s">
         <v>843</v>
       </c>
@@ -41750,7 +41756,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="1099" spans="2:5">
+    <row r="1099" spans="2:7">
       <c r="B1099" t="s">
         <v>843</v>
       </c>
@@ -41764,7 +41770,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="1100" spans="2:5">
+    <row r="1100" spans="2:7">
       <c r="B1100" t="s">
         <v>843</v>
       </c>
@@ -41778,7 +41784,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="1101" spans="2:5">
+    <row r="1101" spans="2:7">
       <c r="B1101" t="s">
         <v>843</v>
       </c>
@@ -41792,7 +41798,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="1102" spans="2:5">
+    <row r="1102" spans="2:7">
       <c r="B1102" t="s">
         <v>843</v>
       </c>
@@ -41806,7 +41812,7 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="1103" spans="2:5">
+    <row r="1103" spans="2:7">
       <c r="B1103" t="s">
         <v>843</v>
       </c>
@@ -41820,7 +41826,7 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="1104" spans="2:5">
+    <row r="1104" spans="2:7">
       <c r="B1104" t="s">
         <v>843</v>
       </c>
@@ -41875,9 +41881,6 @@
       <c r="E1107" t="s">
         <v>1236</v>
       </c>
-      <c r="F1107" t="s">
-        <v>1215</v>
-      </c>
     </row>
     <row r="1108" spans="2:7">
       <c r="B1108" t="s">
@@ -41892,12 +41895,6 @@
       <c r="E1108" s="10" t="s">
         <v>1238</v>
       </c>
-      <c r="F1108" t="s">
-        <v>1217</v>
-      </c>
-      <c r="G1108" t="s">
-        <v>1218</v>
-      </c>
     </row>
     <row r="1109" spans="2:7">
       <c r="B1109" t="s">
@@ -41907,10 +41904,7 @@
         <v>18</v>
       </c>
       <c r="F1109" t="s">
-        <v>1217</v>
-      </c>
-      <c r="G1109" t="s">
-        <v>1389</v>
+        <v>1215</v>
       </c>
     </row>
     <row r="1110" spans="2:7">
@@ -41924,7 +41918,7 @@
         <v>1217</v>
       </c>
       <c r="G1110" t="s">
-        <v>1365</v>
+        <v>1218</v>
       </c>
     </row>
     <row r="1111" spans="2:7">
@@ -41935,10 +41929,10 @@
         <v>850</v>
       </c>
       <c r="F1111" t="s">
-        <v>1230</v>
+        <v>1217</v>
       </c>
       <c r="G1111" t="s">
-        <v>1376</v>
+        <v>1389</v>
       </c>
     </row>
     <row r="1112" spans="2:7">
@@ -41948,6 +41942,12 @@
       <c r="C1112" t="s">
         <v>852</v>
       </c>
+      <c r="F1112" t="s">
+        <v>1217</v>
+      </c>
+      <c r="G1112" t="s">
+        <v>1365</v>
+      </c>
     </row>
     <row r="1113" spans="2:7">
       <c r="B1113" t="s">
@@ -41956,6 +41956,12 @@
       <c r="C1113" t="s">
         <v>854</v>
       </c>
+      <c r="F1113" t="s">
+        <v>1230</v>
+      </c>
+      <c r="G1113" t="s">
+        <v>1376</v>
+      </c>
     </row>
     <row r="1114" spans="2:7">
       <c r="B1114" t="s">
@@ -42055,7 +42061,7 @@
         <v>1369</v>
       </c>
     </row>
-    <row r="1121" spans="2:7">
+    <row r="1121" spans="2:6">
       <c r="B1121" t="s">
         <v>843</v>
       </c>
@@ -42069,7 +42075,7 @@
         <v>1370</v>
       </c>
     </row>
-    <row r="1122" spans="2:7">
+    <row r="1122" spans="2:6">
       <c r="B1122" t="s">
         <v>843</v>
       </c>
@@ -42083,7 +42089,7 @@
         <v>1371</v>
       </c>
     </row>
-    <row r="1123" spans="2:7">
+    <row r="1123" spans="2:6">
       <c r="B1123" t="s">
         <v>843</v>
       </c>
@@ -42097,7 +42103,7 @@
         <v>1372</v>
       </c>
     </row>
-    <row r="1124" spans="2:7">
+    <row r="1124" spans="2:6">
       <c r="B1124" t="s">
         <v>843</v>
       </c>
@@ -42111,7 +42117,7 @@
         <v>1372</v>
       </c>
     </row>
-    <row r="1125" spans="2:7">
+    <row r="1125" spans="2:6">
       <c r="B1125" t="s">
         <v>843</v>
       </c>
@@ -42125,7 +42131,7 @@
         <v>1390</v>
       </c>
     </row>
-    <row r="1126" spans="2:7">
+    <row r="1126" spans="2:6">
       <c r="B1126" t="s">
         <v>843</v>
       </c>
@@ -42139,7 +42145,7 @@
         <v>1391</v>
       </c>
     </row>
-    <row r="1127" spans="2:7">
+    <row r="1127" spans="2:6">
       <c r="B1127" t="s">
         <v>843</v>
       </c>
@@ -42153,7 +42159,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="1128" spans="2:7">
+    <row r="1128" spans="2:6">
       <c r="B1128" t="s">
         <v>843</v>
       </c>
@@ -42167,7 +42173,7 @@
         <v>1393</v>
       </c>
     </row>
-    <row r="1129" spans="2:7">
+    <row r="1129" spans="2:6">
       <c r="B1129" t="s">
         <v>843</v>
       </c>
@@ -42181,7 +42187,7 @@
         <v>1394</v>
       </c>
     </row>
-    <row r="1130" spans="2:7">
+    <row r="1130" spans="2:6">
       <c r="B1130" t="s">
         <v>843</v>
       </c>
@@ -42194,11 +42200,8 @@
       <c r="E1130" s="10" t="s">
         <v>1395</v>
       </c>
-      <c r="F1130" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="1131" spans="2:7">
+    </row>
+    <row r="1131" spans="2:6">
       <c r="B1131" t="s">
         <v>843</v>
       </c>
@@ -42212,15 +42215,18 @@
         <v>1255</v>
       </c>
     </row>
-    <row r="1132" spans="2:7">
+    <row r="1132" spans="2:6">
       <c r="B1132" t="s">
         <v>843</v>
       </c>
       <c r="C1132" t="s">
         <v>862</v>
       </c>
-    </row>
-    <row r="1133" spans="2:7">
+      <c r="F1132" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="1133" spans="2:6">
       <c r="B1133" t="s">
         <v>843</v>
       </c>
@@ -42234,7 +42240,7 @@
         <v>1224</v>
       </c>
     </row>
-    <row r="1134" spans="2:7">
+    <row r="1134" spans="2:6">
       <c r="B1134" t="s">
         <v>843</v>
       </c>
@@ -42247,11 +42253,8 @@
       <c r="E1134" t="s">
         <v>1226</v>
       </c>
-      <c r="F1134" t="s">
-        <v>1215</v>
-      </c>
-    </row>
-    <row r="1135" spans="2:7">
+    </row>
+    <row r="1135" spans="2:6">
       <c r="B1135" t="s">
         <v>843</v>
       </c>
@@ -42264,14 +42267,8 @@
       <c r="E1135" s="10" t="s">
         <v>1399</v>
       </c>
-      <c r="F1135" t="s">
-        <v>1230</v>
-      </c>
-      <c r="G1135" t="s">
-        <v>1376</v>
-      </c>
-    </row>
-    <row r="1136" spans="2:7">
+    </row>
+    <row r="1136" spans="2:6">
       <c r="B1136" t="s">
         <v>843</v>
       </c>
@@ -42353,6 +42350,9 @@
       <c r="C1142" t="s">
         <v>878</v>
       </c>
+      <c r="F1142" t="s">
+        <v>1215</v>
+      </c>
     </row>
     <row r="1143" spans="2:7">
       <c r="B1143" t="s">
@@ -42361,6 +42361,12 @@
       <c r="C1143" t="s">
         <v>880</v>
       </c>
+      <c r="F1143" t="s">
+        <v>1230</v>
+      </c>
+      <c r="G1143" t="s">
+        <v>1376</v>
+      </c>
     </row>
     <row r="1144" spans="2:7">
       <c r="B1144" t="s">
@@ -42417,12 +42423,6 @@
       <c r="E1147" s="10" t="s">
         <v>1399</v>
       </c>
-      <c r="F1147" s="12" t="s">
-        <v>1230</v>
-      </c>
-      <c r="G1147" t="s">
-        <v>1376</v>
-      </c>
     </row>
     <row r="1148" spans="2:7">
       <c r="B1148" t="s">
@@ -42445,6 +42445,12 @@
       <c r="C1149" t="s">
         <v>886</v>
       </c>
+      <c r="F1149" s="12" t="s">
+        <v>1230</v>
+      </c>
+      <c r="G1149" t="s">
+        <v>1376</v>
+      </c>
     </row>
     <row r="1150" spans="2:7">
       <c r="B1150" t="s">
@@ -42501,12 +42507,6 @@
       <c r="E1153" s="10" t="s">
         <v>1399</v>
       </c>
-      <c r="F1153" s="12" t="s">
-        <v>1230</v>
-      </c>
-      <c r="G1153" t="s">
-        <v>1376</v>
-      </c>
     </row>
     <row r="1154" spans="2:7">
       <c r="B1154" t="s">
@@ -42529,6 +42529,12 @@
       <c r="C1155" t="s">
         <v>890</v>
       </c>
+      <c r="F1155" s="12" t="s">
+        <v>1230</v>
+      </c>
+      <c r="G1155" t="s">
+        <v>1376</v>
+      </c>
     </row>
     <row r="1156" spans="2:7">
       <c r="B1156" t="s">
@@ -42585,12 +42591,6 @@
       <c r="E1159" s="10" t="s">
         <v>1399</v>
       </c>
-      <c r="F1159" s="12" t="s">
-        <v>1230</v>
-      </c>
-      <c r="G1159" t="s">
-        <v>1376</v>
-      </c>
     </row>
     <row r="1160" spans="2:7">
       <c r="B1160" t="s">
@@ -42613,6 +42613,12 @@
       <c r="C1161" t="s">
         <v>893</v>
       </c>
+      <c r="F1161" s="12" t="s">
+        <v>1230</v>
+      </c>
+      <c r="G1161" t="s">
+        <v>1376</v>
+      </c>
     </row>
     <row r="1162" spans="2:7">
       <c r="B1162" t="s">
@@ -42669,12 +42675,6 @@
       <c r="E1165" s="10" t="s">
         <v>1399</v>
       </c>
-      <c r="F1165" s="12" t="s">
-        <v>1230</v>
-      </c>
-      <c r="G1165" t="s">
-        <v>1376</v>
-      </c>
     </row>
     <row r="1166" spans="2:7">
       <c r="B1166" t="s">
@@ -42697,6 +42697,12 @@
       <c r="C1167" t="s">
         <v>896</v>
       </c>
+      <c r="F1167" s="12" t="s">
+        <v>1230</v>
+      </c>
+      <c r="G1167" t="s">
+        <v>1376</v>
+      </c>
     </row>
     <row r="1168" spans="2:7">
       <c r="B1168" t="s">
@@ -42753,12 +42759,6 @@
       <c r="E1171" s="10" t="s">
         <v>1399</v>
       </c>
-      <c r="F1171" s="12" t="s">
-        <v>1230</v>
-      </c>
-      <c r="G1171" t="s">
-        <v>1376</v>
-      </c>
     </row>
     <row r="1172" spans="2:7">
       <c r="B1172" t="s">
@@ -42781,6 +42781,12 @@
       <c r="C1173" t="s">
         <v>899</v>
       </c>
+      <c r="F1173" s="12" t="s">
+        <v>1230</v>
+      </c>
+      <c r="G1173" t="s">
+        <v>1376</v>
+      </c>
     </row>
     <row r="1174" spans="2:7">
       <c r="B1174" t="s">
@@ -42837,12 +42843,6 @@
       <c r="E1177" s="10" t="s">
         <v>1399</v>
       </c>
-      <c r="F1177" s="12" t="s">
-        <v>1230</v>
-      </c>
-      <c r="G1177" t="s">
-        <v>1376</v>
-      </c>
     </row>
     <row r="1178" spans="2:7">
       <c r="B1178" t="s">
@@ -42865,6 +42865,12 @@
       <c r="C1179" t="s">
         <v>902</v>
       </c>
+      <c r="F1179" s="12" t="s">
+        <v>1230</v>
+      </c>
+      <c r="G1179" t="s">
+        <v>1376</v>
+      </c>
     </row>
     <row r="1180" spans="2:7">
       <c r="B1180" t="s">
@@ -42921,12 +42927,6 @@
       <c r="E1183" s="10" t="s">
         <v>1399</v>
       </c>
-      <c r="F1183" s="12" t="s">
-        <v>1230</v>
-      </c>
-      <c r="G1183" t="s">
-        <v>1376</v>
-      </c>
     </row>
     <row r="1184" spans="2:7">
       <c r="B1184" t="s">
@@ -42949,6 +42949,12 @@
       <c r="C1185" t="s">
         <v>905</v>
       </c>
+      <c r="F1185" s="12" t="s">
+        <v>1230</v>
+      </c>
+      <c r="G1185" t="s">
+        <v>1376</v>
+      </c>
     </row>
     <row r="1186" spans="2:7">
       <c r="B1186" t="s">
@@ -43005,12 +43011,6 @@
       <c r="E1189" s="10" t="s">
         <v>1399</v>
       </c>
-      <c r="F1189" s="12" t="s">
-        <v>1230</v>
-      </c>
-      <c r="G1189" t="s">
-        <v>1376</v>
-      </c>
     </row>
     <row r="1190" spans="2:7">
       <c r="B1190" t="s">
@@ -43033,6 +43033,12 @@
       <c r="C1191" t="s">
         <v>908</v>
       </c>
+      <c r="F1191" s="12" t="s">
+        <v>1230</v>
+      </c>
+      <c r="G1191" t="s">
+        <v>1376</v>
+      </c>
     </row>
     <row r="1192" spans="2:7">
       <c r="B1192" t="s">
@@ -43089,12 +43095,6 @@
       <c r="E1195" s="10" t="s">
         <v>1399</v>
       </c>
-      <c r="F1195" s="12" t="s">
-        <v>1230</v>
-      </c>
-      <c r="G1195" t="s">
-        <v>1376</v>
-      </c>
     </row>
     <row r="1196" spans="2:7">
       <c r="B1196" t="s">
@@ -43117,6 +43117,12 @@
       <c r="C1197" t="s">
         <v>911</v>
       </c>
+      <c r="F1197" s="12" t="s">
+        <v>1230</v>
+      </c>
+      <c r="G1197" t="s">
+        <v>1376</v>
+      </c>
     </row>
     <row r="1198" spans="2:7">
       <c r="B1198" t="s">
@@ -43173,12 +43179,6 @@
       <c r="E1201" s="10" t="s">
         <v>1399</v>
       </c>
-      <c r="F1201" s="12" t="s">
-        <v>1230</v>
-      </c>
-      <c r="G1201" t="s">
-        <v>1376</v>
-      </c>
     </row>
     <row r="1202" spans="2:7">
       <c r="B1202" t="s">
@@ -43193,9 +43193,6 @@
       <c r="E1202" s="10" t="s">
         <v>1236</v>
       </c>
-      <c r="F1202" t="s">
-        <v>184</v>
-      </c>
     </row>
     <row r="1203" spans="2:7">
       <c r="B1203" t="s">
@@ -43204,8 +43201,11 @@
       <c r="C1203" t="s">
         <v>914</v>
       </c>
-      <c r="F1203" t="s">
-        <v>184</v>
+      <c r="F1203" s="12" t="s">
+        <v>1230</v>
+      </c>
+      <c r="G1203" t="s">
+        <v>1376</v>
       </c>
     </row>
     <row r="1204" spans="2:7">
@@ -43226,6 +43226,9 @@
       <c r="C1205" t="s">
         <v>917</v>
       </c>
+      <c r="F1205" t="s">
+        <v>184</v>
+      </c>
     </row>
     <row r="1206" spans="2:7">
       <c r="B1206" t="s">
@@ -43234,6 +43237,9 @@
       <c r="C1206" t="s">
         <v>919</v>
       </c>
+      <c r="F1206" t="s">
+        <v>184</v>
+      </c>
     </row>
     <row r="1207" spans="2:7">
       <c r="B1207" t="s">
@@ -43304,9 +43310,6 @@
       <c r="E1211" t="s">
         <v>1236</v>
       </c>
-      <c r="F1211" t="s">
-        <v>184</v>
-      </c>
     </row>
     <row r="1212" spans="2:7">
       <c r="B1212" t="s">
@@ -43329,6 +43332,9 @@
       <c r="C1213" t="s">
         <v>927</v>
       </c>
+      <c r="F1213" t="s">
+        <v>184</v>
+      </c>
     </row>
     <row r="1214" spans="2:7">
       <c r="B1214" t="s">
@@ -43399,9 +43405,6 @@
       <c r="E1218" t="s">
         <v>1236</v>
       </c>
-      <c r="F1218" t="s">
-        <v>184</v>
-      </c>
     </row>
     <row r="1219" spans="2:6">
       <c r="B1219" t="s">
@@ -43424,6 +43427,9 @@
       <c r="C1220" t="s">
         <v>931</v>
       </c>
+      <c r="F1220" t="s">
+        <v>184</v>
+      </c>
     </row>
     <row r="1221" spans="2:6">
       <c r="B1221" t="s">
@@ -43494,9 +43500,6 @@
       <c r="E1225" t="s">
         <v>1236</v>
       </c>
-      <c r="F1225" t="s">
-        <v>184</v>
-      </c>
     </row>
     <row r="1226" spans="2:6">
       <c r="B1226" t="s">
@@ -43519,6 +43522,9 @@
       <c r="C1227" t="s">
         <v>935</v>
       </c>
+      <c r="F1227" t="s">
+        <v>184</v>
+      </c>
     </row>
     <row r="1228" spans="2:6">
       <c r="B1228" t="s">
@@ -43589,9 +43595,6 @@
       <c r="E1232" t="s">
         <v>1236</v>
       </c>
-      <c r="F1232" t="s">
-        <v>184</v>
-      </c>
     </row>
     <row r="1233" spans="2:6">
       <c r="B1233" t="s">
@@ -43614,6 +43617,9 @@
       <c r="C1234" t="s">
         <v>939</v>
       </c>
+      <c r="F1234" t="s">
+        <v>184</v>
+      </c>
     </row>
     <row r="1235" spans="2:6">
       <c r="B1235" t="s">
@@ -43684,9 +43690,6 @@
       <c r="E1239" t="s">
         <v>1236</v>
       </c>
-      <c r="F1239" t="s">
-        <v>184</v>
-      </c>
     </row>
     <row r="1240" spans="2:6">
       <c r="B1240" t="s">
@@ -43709,6 +43712,9 @@
       <c r="C1241" t="s">
         <v>943</v>
       </c>
+      <c r="F1241" t="s">
+        <v>184</v>
+      </c>
     </row>
     <row r="1242" spans="2:6">
       <c r="B1242" t="s">
@@ -43807,9 +43813,6 @@
       <c r="E1248" t="s">
         <v>1236</v>
       </c>
-      <c r="F1248" t="s">
-        <v>184</v>
-      </c>
     </row>
     <row r="1249" spans="2:7">
       <c r="B1249" t="s">
@@ -43832,6 +43835,9 @@
       <c r="C1250" t="s">
         <v>949</v>
       </c>
+      <c r="F1250" t="s">
+        <v>184</v>
+      </c>
     </row>
     <row r="1251" spans="2:7">
       <c r="B1251" t="s">
@@ -43846,9 +43852,6 @@
       <c r="E1251" s="10" t="s">
         <v>1238</v>
       </c>
-      <c r="F1251" t="s">
-        <v>184</v>
-      </c>
     </row>
     <row r="1252" spans="2:7">
       <c r="B1252" t="s">
@@ -43863,9 +43866,6 @@
       <c r="E1252" t="s">
         <v>1236</v>
       </c>
-      <c r="F1252" t="s">
-        <v>184</v>
-      </c>
     </row>
     <row r="1253" spans="2:7">
       <c r="B1253" t="s">
@@ -43930,10 +43930,7 @@
         <v>962</v>
       </c>
       <c r="F1258" t="s">
-        <v>1217</v>
-      </c>
-      <c r="G1258" t="s">
-        <v>1240</v>
+        <v>184</v>
       </c>
     </row>
     <row r="1259" spans="2:7">
@@ -43944,10 +43941,7 @@
         <v>964</v>
       </c>
       <c r="F1259" t="s">
-        <v>1217</v>
-      </c>
-      <c r="G1259" t="s">
-        <v>1297</v>
+        <v>184</v>
       </c>
     </row>
     <row r="1260" spans="2:7">
@@ -43961,7 +43955,7 @@
         <v>1217</v>
       </c>
       <c r="G1260" t="s">
-        <v>1297</v>
+        <v>1240</v>
       </c>
     </row>
     <row r="1261" spans="2:7">
@@ -44070,7 +44064,10 @@
         <v>975</v>
       </c>
       <c r="F1268" t="s">
-        <v>184</v>
+        <v>1217</v>
+      </c>
+      <c r="G1268" t="s">
+        <v>1297</v>
       </c>
     </row>
     <row r="1269" spans="2:7">
@@ -44081,7 +44078,10 @@
         <v>976</v>
       </c>
       <c r="F1269" t="s">
-        <v>184</v>
+        <v>1217</v>
+      </c>
+      <c r="G1269" t="s">
+        <v>1297</v>
       </c>
     </row>
     <row r="1270" spans="2:7">
@@ -44245,6 +44245,9 @@
       <c r="C1284" t="s">
         <v>1041</v>
       </c>
+      <c r="F1284" t="s">
+        <v>184</v>
+      </c>
     </row>
     <row r="1285" spans="2:6">
       <c r="B1285" t="s">
@@ -44253,6 +44256,9 @@
       <c r="C1285" t="s">
         <v>1047</v>
       </c>
+      <c r="F1285" t="s">
+        <v>184</v>
+      </c>
     </row>
     <row r="1286" spans="2:6">
       <c r="B1286" t="s">
@@ -44659,12 +44665,6 @@
       <c r="E1314" t="s">
         <v>1226</v>
       </c>
-      <c r="F1314" t="s">
-        <v>1217</v>
-      </c>
-      <c r="G1314" t="s">
-        <v>1240</v>
-      </c>
     </row>
     <row r="1315" spans="2:7">
       <c r="B1315" t="s">
@@ -44679,12 +44679,6 @@
       <c r="E1315" s="10" t="s">
         <v>1399</v>
       </c>
-      <c r="F1315" t="s">
-        <v>1217</v>
-      </c>
-      <c r="G1315" t="s">
-        <v>1240</v>
-      </c>
     </row>
     <row r="1316" spans="2:7">
       <c r="B1316" t="s">
@@ -44806,7 +44800,10 @@
         <v>1043</v>
       </c>
       <c r="F1324" t="s">
-        <v>184</v>
+        <v>1217</v>
+      </c>
+      <c r="G1324" t="s">
+        <v>1240</v>
       </c>
     </row>
     <row r="1325" spans="2:7">
@@ -44817,7 +44814,10 @@
         <v>1049</v>
       </c>
       <c r="F1325" t="s">
-        <v>184</v>
+        <v>1217</v>
+      </c>
+      <c r="G1325" t="s">
+        <v>1240</v>
       </c>
     </row>
     <row r="1326" spans="2:7">
@@ -44915,6 +44915,9 @@
       <c r="C1334" t="s">
         <v>1044</v>
       </c>
+      <c r="F1334" t="s">
+        <v>184</v>
+      </c>
     </row>
     <row r="1335" spans="2:6">
       <c r="B1335" t="s">
@@ -44923,6 +44926,9 @@
       <c r="C1335" t="s">
         <v>1050</v>
       </c>
+      <c r="F1335" t="s">
+        <v>184</v>
+      </c>
     </row>
     <row r="1336" spans="2:6">
       <c r="B1336" t="s">
@@ -45189,9 +45195,6 @@
       <c r="E1354" t="s">
         <v>1404</v>
       </c>
-      <c r="F1354" t="s">
-        <v>184</v>
-      </c>
     </row>
     <row r="1355" spans="2:6">
       <c r="B1355" t="s">
@@ -45206,9 +45209,6 @@
       <c r="E1355" t="s">
         <v>1404</v>
       </c>
-      <c r="F1355" t="s">
-        <v>184</v>
-      </c>
     </row>
     <row r="1356" spans="2:6">
       <c r="B1356" t="s">
@@ -45306,10 +45306,7 @@
         <v>1046</v>
       </c>
       <c r="F1364" t="s">
-        <v>1217</v>
-      </c>
-      <c r="G1364" t="s">
-        <v>1297</v>
+        <v>184</v>
       </c>
     </row>
     <row r="1365" spans="2:7">
@@ -45320,10 +45317,7 @@
         <v>1052</v>
       </c>
       <c r="F1365" t="s">
-        <v>1217</v>
-      </c>
-      <c r="G1365" t="s">
-        <v>1297</v>
+        <v>184</v>
       </c>
     </row>
     <row r="1366" spans="2:7">
@@ -45390,7 +45384,10 @@
         <v>1061</v>
       </c>
       <c r="F1370" t="s">
-        <v>184</v>
+        <v>1217</v>
+      </c>
+      <c r="G1370" t="s">
+        <v>1297</v>
       </c>
     </row>
     <row r="1371" spans="2:7">
@@ -45401,7 +45398,10 @@
         <v>1063</v>
       </c>
       <c r="F1371" t="s">
-        <v>184</v>
+        <v>1217</v>
+      </c>
+      <c r="G1371" t="s">
+        <v>1297</v>
       </c>
     </row>
     <row r="1372" spans="2:7">
@@ -45411,6 +45411,9 @@
       <c r="C1372" t="s">
         <v>1065</v>
       </c>
+      <c r="F1372" t="s">
+        <v>184</v>
+      </c>
     </row>
     <row r="1373" spans="2:7">
       <c r="B1373" t="s">
@@ -45419,6 +45422,9 @@
       <c r="C1373" t="s">
         <v>1067</v>
       </c>
+      <c r="F1373" t="s">
+        <v>184</v>
+      </c>
     </row>
     <row r="1374" spans="2:7">
       <c r="B1374" t="s">
@@ -45433,9 +45439,6 @@
       <c r="E1374" t="s">
         <v>1236</v>
       </c>
-      <c r="F1374" t="s">
-        <v>184</v>
-      </c>
     </row>
     <row r="1375" spans="2:7">
       <c r="B1375" t="s">
@@ -45450,9 +45453,6 @@
       <c r="E1375" s="10" t="s">
         <v>1238</v>
       </c>
-      <c r="F1375" t="s">
-        <v>184</v>
-      </c>
     </row>
     <row r="1376" spans="2:7">
       <c r="B1376" t="s">
@@ -45494,6 +45494,9 @@
       <c r="C1379" t="s">
         <v>1076</v>
       </c>
+      <c r="F1379" t="s">
+        <v>184</v>
+      </c>
     </row>
     <row r="1380" spans="2:6">
       <c r="B1380" t="s">
@@ -45502,6 +45505,9 @@
       <c r="C1380" t="s">
         <v>1078</v>
       </c>
+      <c r="F1380" t="s">
+        <v>184</v>
+      </c>
     </row>
     <row r="1381" spans="2:6">
       <c r="B1381" t="s">
@@ -45516,9 +45522,6 @@
       <c r="E1381" t="s">
         <v>1236</v>
       </c>
-      <c r="F1381" t="s">
-        <v>184</v>
-      </c>
     </row>
     <row r="1382" spans="2:6">
       <c r="B1382" t="s">
@@ -45541,6 +45544,9 @@
       <c r="C1383" t="s">
         <v>1082</v>
       </c>
+      <c r="F1383" t="s">
+        <v>184</v>
+      </c>
     </row>
     <row r="1384" spans="2:6">
       <c r="B1384" t="s">
@@ -45555,9 +45561,6 @@
       <c r="E1384" t="s">
         <v>1236</v>
       </c>
-      <c r="F1384" t="s">
-        <v>184</v>
-      </c>
     </row>
     <row r="1385" spans="2:6">
       <c r="B1385" t="s">
@@ -45580,6 +45583,9 @@
       <c r="C1386" t="s">
         <v>1086</v>
       </c>
+      <c r="F1386" t="s">
+        <v>184</v>
+      </c>
     </row>
     <row r="1387" spans="2:6">
       <c r="B1387" t="s">
@@ -45594,9 +45600,6 @@
       <c r="E1387" t="s">
         <v>1236</v>
       </c>
-      <c r="F1387" t="s">
-        <v>184</v>
-      </c>
     </row>
     <row r="1388" spans="2:6">
       <c r="B1388" t="s">
@@ -45611,9 +45614,6 @@
       <c r="E1388" s="10" t="s">
         <v>1238</v>
       </c>
-      <c r="F1388" t="s">
-        <v>184</v>
-      </c>
     </row>
     <row r="1389" spans="2:6">
       <c r="B1389" t="s">
@@ -45644,6 +45644,9 @@
       <c r="C1391" t="s">
         <v>1094</v>
       </c>
+      <c r="F1391" t="s">
+        <v>184</v>
+      </c>
     </row>
     <row r="1392" spans="2:6">
       <c r="B1392" t="s">
@@ -45652,6 +45655,9 @@
       <c r="C1392" t="s">
         <v>1096</v>
       </c>
+      <c r="F1392" t="s">
+        <v>184</v>
+      </c>
     </row>
     <row r="1393" spans="2:6">
       <c r="B1393" t="s">
@@ -45708,9 +45714,6 @@
       <c r="E1396" s="10" t="s">
         <v>1408</v>
       </c>
-      <c r="F1396" t="s">
-        <v>1217</v>
-      </c>
     </row>
     <row r="1397" spans="2:6">
       <c r="B1397" t="s">
@@ -45725,9 +45728,6 @@
       <c r="E1397" s="10" t="s">
         <v>1409</v>
       </c>
-      <c r="F1397" t="s">
-        <v>1215</v>
-      </c>
     </row>
     <row r="1398" spans="2:6">
       <c r="B1398" t="s">
@@ -45748,7 +45748,7 @@
         <v>1102</v>
       </c>
       <c r="F1399" t="s">
-        <v>1217</v>
+        <v>1215</v>
       </c>
     </row>
     <row r="1400" spans="2:6">
@@ -45759,7 +45759,7 @@
         <v>1104</v>
       </c>
       <c r="F1400" t="s">
-        <v>1215</v>
+        <v>1217</v>
       </c>
     </row>
     <row r="1401" spans="2:6">
@@ -45770,7 +45770,7 @@
         <v>1106</v>
       </c>
       <c r="F1401" t="s">
-        <v>1215</v>
+        <v>1217</v>
       </c>
     </row>
     <row r="1402" spans="2:6">
@@ -45803,7 +45803,7 @@
         <v>1111</v>
       </c>
       <c r="F1404" t="s">
-        <v>1217</v>
+        <v>1215</v>
       </c>
     </row>
     <row r="1405" spans="2:6">
@@ -45825,7 +45825,7 @@
         <v>1114</v>
       </c>
       <c r="F1406" t="s">
-        <v>1215</v>
+        <v>1217</v>
       </c>
     </row>
     <row r="1407" spans="2:6">
@@ -45913,10 +45913,7 @@
         <v>1180</v>
       </c>
       <c r="F1414" t="s">
-        <v>1217</v>
-      </c>
-      <c r="G1414" t="s">
-        <v>1240</v>
+        <v>1215</v>
       </c>
     </row>
     <row r="1415" spans="2:7">
@@ -45927,10 +45924,7 @@
         <v>1410</v>
       </c>
       <c r="F1415" t="s">
-        <v>1217</v>
-      </c>
-      <c r="G1415" t="s">
-        <v>1240</v>
+        <v>1215</v>
       </c>
     </row>
     <row r="1416" spans="2:7">
@@ -46038,6 +46032,12 @@
       <c r="C1423" t="s">
         <v>1181</v>
       </c>
+      <c r="F1423" t="s">
+        <v>1217</v>
+      </c>
+      <c r="G1423" t="s">
+        <v>1240</v>
+      </c>
     </row>
     <row r="1424" spans="2:7">
       <c r="B1424" t="s">
@@ -46046,6 +46046,12 @@
       <c r="C1424" t="s">
         <v>1411</v>
       </c>
+      <c r="F1424" t="s">
+        <v>1217</v>
+      </c>
+      <c r="G1424" t="s">
+        <v>1240</v>
+      </c>
     </row>
     <row r="1425" spans="2:5">
       <c r="B1425" t="s">
@@ -46410,9 +46416,6 @@
       <c r="E1450" s="10" t="s">
         <v>1399</v>
       </c>
-      <c r="F1450" t="s">
-        <v>184</v>
-      </c>
     </row>
     <row r="1451" spans="2:6">
       <c r="B1451" t="s">
@@ -46427,9 +46430,6 @@
       <c r="E1451" s="10" t="s">
         <v>1399</v>
       </c>
-      <c r="F1451" t="s">
-        <v>184</v>
-      </c>
     </row>
     <row r="1452" spans="2:6">
       <c r="B1452" t="s">
@@ -46516,7 +46516,7 @@
         <v>1183</v>
       </c>
       <c r="F1459" t="s">
-        <v>1217</v>
+        <v>184</v>
       </c>
     </row>
     <row r="1460" spans="2:6">
@@ -46527,7 +46527,7 @@
         <v>1413</v>
       </c>
       <c r="F1460" t="s">
-        <v>1217</v>
+        <v>184</v>
       </c>
     </row>
     <row r="1461" spans="2:6">
@@ -46614,6 +46614,9 @@
       <c r="C1468" t="s">
         <v>1184</v>
       </c>
+      <c r="F1468" t="s">
+        <v>1217</v>
+      </c>
     </row>
     <row r="1469" spans="2:6">
       <c r="B1469" t="s">
@@ -46622,6 +46625,9 @@
       <c r="C1469" t="s">
         <v>1414</v>
       </c>
+      <c r="F1469" t="s">
+        <v>1217</v>
+      </c>
     </row>
     <row r="1470" spans="2:6">
       <c r="B1470" t="s">
@@ -46889,7 +46895,7 @@
         <v>1236</v>
       </c>
     </row>
-    <row r="1489" spans="2:7">
+    <row r="1489" spans="2:5">
       <c r="B1489" t="s">
         <v>843</v>
       </c>
@@ -46903,7 +46909,7 @@
         <v>1236</v>
       </c>
     </row>
-    <row r="1490" spans="2:7">
+    <row r="1490" spans="2:5">
       <c r="B1490" t="s">
         <v>843</v>
       </c>
@@ -46917,7 +46923,7 @@
         <v>1236</v>
       </c>
     </row>
-    <row r="1491" spans="2:7">
+    <row r="1491" spans="2:5">
       <c r="B1491" t="s">
         <v>843</v>
       </c>
@@ -46931,7 +46937,7 @@
         <v>1236</v>
       </c>
     </row>
-    <row r="1492" spans="2:7">
+    <row r="1492" spans="2:5">
       <c r="B1492" t="s">
         <v>843</v>
       </c>
@@ -46945,7 +46951,7 @@
         <v>1236</v>
       </c>
     </row>
-    <row r="1493" spans="2:7">
+    <row r="1493" spans="2:5">
       <c r="B1493" t="s">
         <v>843</v>
       </c>
@@ -46959,7 +46965,7 @@
         <v>1236</v>
       </c>
     </row>
-    <row r="1494" spans="2:7">
+    <row r="1494" spans="2:5">
       <c r="B1494" t="s">
         <v>843</v>
       </c>
@@ -46973,7 +46979,7 @@
         <v>1236</v>
       </c>
     </row>
-    <row r="1495" spans="2:7">
+    <row r="1495" spans="2:5">
       <c r="B1495" t="s">
         <v>843</v>
       </c>
@@ -46987,7 +46993,7 @@
         <v>1236</v>
       </c>
     </row>
-    <row r="1496" spans="2:7">
+    <row r="1496" spans="2:5">
       <c r="B1496" t="s">
         <v>843</v>
       </c>
@@ -47001,7 +47007,7 @@
         <v>1236</v>
       </c>
     </row>
-    <row r="1497" spans="2:7">
+    <row r="1497" spans="2:5">
       <c r="B1497" t="s">
         <v>843</v>
       </c>
@@ -47015,7 +47021,7 @@
         <v>1238</v>
       </c>
     </row>
-    <row r="1498" spans="2:7">
+    <row r="1498" spans="2:5">
       <c r="B1498" t="s">
         <v>843</v>
       </c>
@@ -47029,7 +47035,7 @@
         <v>1238</v>
       </c>
     </row>
-    <row r="1499" spans="2:7">
+    <row r="1499" spans="2:5">
       <c r="B1499" t="s">
         <v>843</v>
       </c>
@@ -47043,7 +47049,7 @@
         <v>1238</v>
       </c>
     </row>
-    <row r="1500" spans="2:7">
+    <row r="1500" spans="2:5">
       <c r="B1500" t="s">
         <v>843</v>
       </c>
@@ -47057,7 +47063,7 @@
         <v>1238</v>
       </c>
     </row>
-    <row r="1501" spans="2:7">
+    <row r="1501" spans="2:5">
       <c r="B1501" t="s">
         <v>843</v>
       </c>
@@ -47071,7 +47077,7 @@
         <v>1238</v>
       </c>
     </row>
-    <row r="1502" spans="2:7">
+    <row r="1502" spans="2:5">
       <c r="B1502" t="s">
         <v>843</v>
       </c>
@@ -47085,7 +47091,7 @@
         <v>1238</v>
       </c>
     </row>
-    <row r="1503" spans="2:7">
+    <row r="1503" spans="2:5">
       <c r="B1503" t="s">
         <v>843</v>
       </c>
@@ -47099,7 +47105,7 @@
         <v>1238</v>
       </c>
     </row>
-    <row r="1504" spans="2:7">
+    <row r="1504" spans="2:5">
       <c r="B1504" t="s">
         <v>843</v>
       </c>
@@ -47111,12 +47117,6 @@
       </c>
       <c r="E1504" s="10" t="s">
         <v>1238</v>
-      </c>
-      <c r="F1504" t="s">
-        <v>1217</v>
-      </c>
-      <c r="G1504" t="s">
-        <v>1417</v>
       </c>
     </row>
     <row r="1505" spans="2:7">
@@ -47132,12 +47132,6 @@
       <c r="E1505" s="10" t="s">
         <v>1238</v>
       </c>
-      <c r="F1505" t="s">
-        <v>1217</v>
-      </c>
-      <c r="G1505" t="s">
-        <v>1417</v>
-      </c>
     </row>
     <row r="1506" spans="2:7">
       <c r="B1506" t="s">
@@ -47247,6 +47241,9 @@
       <c r="F1513" t="s">
         <v>1217</v>
       </c>
+      <c r="G1513" t="s">
+        <v>1417</v>
+      </c>
     </row>
     <row r="1514" spans="2:7">
       <c r="B1514" t="s">
@@ -47256,7 +47253,10 @@
         <v>1418</v>
       </c>
       <c r="F1514" t="s">
-        <v>184</v>
+        <v>1217</v>
+      </c>
+      <c r="G1514" t="s">
+        <v>1417</v>
       </c>
     </row>
     <row r="1515" spans="2:7">
@@ -47267,7 +47267,7 @@
         <v>1188</v>
       </c>
       <c r="F1515" t="s">
-        <v>184</v>
+        <v>1217</v>
       </c>
     </row>
     <row r="1516" spans="2:7">
@@ -47365,6 +47365,9 @@
       <c r="C1524" t="s">
         <v>1202</v>
       </c>
+      <c r="F1524" t="s">
+        <v>184</v>
+      </c>
     </row>
     <row r="1525" spans="2:6">
       <c r="B1525" t="s">
@@ -47373,9 +47376,12 @@
       <c r="C1525" t="s">
         <v>1204</v>
       </c>
+      <c r="F1525" t="s">
+        <v>184</v>
+      </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:H1523"/>
+  <autoFilter ref="A1:H1525"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>

</xml_diff>